<commit_message>
Rectification de la note du sprint 2
</commit_message>
<xml_diff>
--- a/Equipe201.xlsx
+++ b/Equipe201.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24722"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikolay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="8_{50A2320D-A701-4D43-9EC9-8C1EC60D081B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E63BFAC1-07F8-40B2-86D2-7D2D39726A2E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CE4B01B-CF11-4340-A426-BBA10F28608F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="194">
   <si>
     <t>Fonct.</t>
   </si>
@@ -600,6 +600,9 @@
   </si>
   <si>
     <t>2.10 Commande réserve</t>
+  </si>
+  <si>
+    <t>Les tests freezent parfois</t>
   </si>
   <si>
     <t>Ne build pas</t>
@@ -1460,7 +1463,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="289">
+  <cellXfs count="290">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2135,6 +2138,9 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2320,13 +2326,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="6" builtinId="39"/>
-    <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="40 % - Accent2" xfId="5" builtinId="35"/>
+    <cellStyle name="40 % - Accent3" xfId="6" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="3" builtinId="21"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
+    <cellStyle name="Sortie" xfId="3" builtinId="21"/>
+    <cellStyle name="Texte explicatif" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2710,7 +2716,7 @@
   <dimension ref="A3:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2773,7 +2779,7 @@
       </c>
       <c r="B5" s="216">
         <f>(Fonctionnalités!E36)</f>
-        <v>0.49400000000000005</v>
+        <v>0.5515000000000001</v>
       </c>
       <c r="C5" s="217">
         <f>'Assurance Qualité'!F61</f>
@@ -2781,14 +2787,14 @@
       </c>
       <c r="D5" s="217">
         <f t="shared" ref="D5:D6" si="0">B5*0.6+C5*0.4 - 0.1*E5</f>
-        <v>0.60760000000000014</v>
+        <v>0.64210000000000012</v>
       </c>
       <c r="F5" s="13">
         <v>25</v>
       </c>
       <c r="G5" s="12">
         <f t="shared" ref="G5:G7" si="1">D5*F5</f>
-        <v>15.190000000000003</v>
+        <v>16.052500000000002</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2861,36 +2867,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A2" s="249" t="s">
+      <c r="A2" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249"/>
-      <c r="H2" s="249"/>
-      <c r="I2" s="249"/>
-      <c r="J2" s="249"/>
-      <c r="K2" s="249"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="250"/>
+      <c r="G2" s="250"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="250"/>
+      <c r="J2" s="250"/>
+      <c r="K2" s="250"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="251" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="250"/>
-      <c r="C4" s="250"/>
-      <c r="D4" s="250"/>
-      <c r="E4" s="250"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="250"/>
-      <c r="H4" s="250"/>
-      <c r="I4" s="250"/>
-      <c r="J4" s="250"/>
-      <c r="K4" s="250"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
@@ -2910,36 +2916,36 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:17" ht="18.399999999999999" customHeight="1">
-      <c r="A6" s="242" t="s">
+      <c r="A6" s="243" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="254" t="s">
+      <c r="B6" s="255" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="244" t="s">
+      <c r="C6" s="245" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="245"/>
-      <c r="E6" s="245"/>
-      <c r="F6" s="246" t="s">
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
+      <c r="F6" s="247" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="247"/>
-      <c r="H6" s="248"/>
-      <c r="I6" s="251" t="s">
+      <c r="G6" s="248"/>
+      <c r="H6" s="249"/>
+      <c r="I6" s="252" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="252"/>
-      <c r="K6" s="253"/>
+      <c r="J6" s="253"/>
+      <c r="K6" s="254"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="240"/>
-      <c r="O6" s="241"/>
-      <c r="P6" s="241"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="242"/>
+      <c r="P6" s="242"/>
     </row>
     <row r="7" spans="1:17" ht="19.5" thickBot="1">
-      <c r="A7" s="243"/>
-      <c r="B7" s="255"/>
+      <c r="A7" s="244"/>
+      <c r="B7" s="256"/>
       <c r="C7" s="22" t="s">
         <v>14</v>
       </c>
@@ -2975,26 +2981,26 @@
       <c r="Q7" s="221"/>
     </row>
     <row r="8" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A8" s="232" t="s">
+      <c r="A8" s="233" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="233"/>
-      <c r="C8" s="228" t="s">
+      <c r="B8" s="234"/>
+      <c r="C8" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="229"/>
+      <c r="D8" s="230"/>
       <c r="E8" s="60"/>
-      <c r="F8" s="228" t="s">
+      <c r="F8" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="229"/>
+      <c r="G8" s="230"/>
       <c r="H8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="228" t="s">
+      <c r="I8" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="229"/>
+      <c r="J8" s="230"/>
       <c r="K8" s="60"/>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
@@ -3159,10 +3165,10 @@
       <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:17" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A14" s="230" t="s">
+      <c r="A14" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="231"/>
+      <c r="B14" s="232"/>
       <c r="C14" s="87">
         <f>SUMPRODUCT(C9:C13,D9:D13)</f>
         <v>9.5</v>
@@ -3194,26 +3200,26 @@
       <c r="M14" s="96"/>
     </row>
     <row r="15" spans="1:17" s="20" customFormat="1" ht="18.399999999999999" customHeight="1">
-      <c r="A15" s="237" t="s">
+      <c r="A15" s="238" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="238"/>
-      <c r="C15" s="228" t="s">
+      <c r="B15" s="239"/>
+      <c r="C15" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="229"/>
+      <c r="D15" s="230"/>
       <c r="E15" s="60"/>
-      <c r="F15" s="228" t="s">
+      <c r="F15" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="229"/>
+      <c r="G15" s="230"/>
       <c r="H15" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="228" t="s">
+      <c r="I15" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="229"/>
+      <c r="J15" s="230"/>
       <c r="K15" s="60"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
@@ -3370,10 +3376,10 @@
       <c r="M20" s="6"/>
     </row>
     <row r="21" spans="1:13" s="97" customFormat="1" ht="15.75">
-      <c r="A21" s="239" t="s">
+      <c r="A21" s="240" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="236"/>
+      <c r="B21" s="237"/>
       <c r="C21" s="98">
         <f>SUMPRODUCT(C16:C20,D16:D20)</f>
         <v>12.7</v>
@@ -3405,26 +3411,26 @@
       <c r="M21" s="96"/>
     </row>
     <row r="22" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A22" s="232" t="s">
+      <c r="A22" s="233" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="233"/>
-      <c r="C22" s="228" t="s">
+      <c r="B22" s="234"/>
+      <c r="C22" s="229" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="229"/>
+      <c r="D22" s="230"/>
       <c r="E22" s="60"/>
-      <c r="F22" s="228" t="s">
+      <c r="F22" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G22" s="229"/>
+      <c r="G22" s="230"/>
       <c r="H22" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I22" s="228" t="s">
+      <c r="I22" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J22" s="229"/>
+      <c r="J22" s="230"/>
       <c r="K22" s="60"/>
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
@@ -3523,10 +3529,10 @@
       <c r="M25" s="6"/>
     </row>
     <row r="26" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A26" s="235" t="s">
+      <c r="A26" s="236" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="236"/>
+      <c r="B26" s="237"/>
       <c r="C26" s="87">
         <f>SUMPRODUCT(C23:C25,D23:D25)</f>
         <v>2</v>
@@ -3558,26 +3564,26 @@
       <c r="M26" s="96"/>
     </row>
     <row r="27" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A27" s="232" t="s">
+      <c r="A27" s="233" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="233"/>
-      <c r="C27" s="228" t="s">
+      <c r="B27" s="234"/>
+      <c r="C27" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="229"/>
+      <c r="D27" s="230"/>
       <c r="E27" s="60"/>
-      <c r="F27" s="228" t="s">
+      <c r="F27" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="229"/>
+      <c r="G27" s="230"/>
       <c r="H27" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="228" t="s">
+      <c r="I27" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="229"/>
+      <c r="J27" s="230"/>
       <c r="K27" s="60"/>
       <c r="L27" s="16"/>
       <c r="M27" s="5"/>
@@ -3705,10 +3711,10 @@
       <c r="M31" s="6"/>
     </row>
     <row r="32" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A32" s="230" t="s">
+      <c r="A32" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="231"/>
+      <c r="B32" s="232"/>
       <c r="C32" s="87">
         <f>SUMPRODUCT(C28:C31,D28:D31)</f>
         <v>6</v>
@@ -3740,19 +3746,19 @@
       <c r="M32" s="96"/>
     </row>
     <row r="33" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A33" s="232" t="s">
+      <c r="A33" s="233" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="234"/>
-      <c r="C33" s="228" t="s">
+      <c r="B33" s="235"/>
+      <c r="C33" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="229"/>
+      <c r="D33" s="230"/>
       <c r="E33" s="60"/>
-      <c r="F33" s="228" t="s">
+      <c r="F33" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="229"/>
+      <c r="G33" s="230"/>
       <c r="H33" s="60" t="s">
         <v>18</v>
       </c>
@@ -3887,10 +3893,10 @@
       <c r="M37" s="6"/>
     </row>
     <row r="38" spans="1:13" s="97" customFormat="1" ht="15.75">
-      <c r="A38" s="230" t="s">
+      <c r="A38" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="231"/>
+      <c r="B38" s="232"/>
       <c r="C38" s="122">
         <f>SUMPRODUCT(C34:C37,D34:D37)</f>
         <v>6.8</v>
@@ -3922,26 +3928,26 @@
       <c r="M38" s="96"/>
     </row>
     <row r="39" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A39" s="232" t="s">
+      <c r="A39" s="233" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="233"/>
-      <c r="C39" s="228" t="s">
+      <c r="B39" s="234"/>
+      <c r="C39" s="229" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="229"/>
+      <c r="D39" s="230"/>
       <c r="E39" s="59"/>
-      <c r="F39" s="228" t="s">
+      <c r="F39" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="229"/>
+      <c r="G39" s="230"/>
       <c r="H39" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="228" t="s">
+      <c r="I39" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="229"/>
+      <c r="J39" s="230"/>
       <c r="K39" s="60"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
@@ -4287,10 +4293,10 @@
       <c r="M50" s="6"/>
     </row>
     <row r="51" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A51" s="230" t="s">
+      <c r="A51" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="231"/>
+      <c r="B51" s="232"/>
       <c r="C51" s="132">
         <f>SUMPRODUCT(C40:C50,D40:D50)</f>
         <v>25.5</v>
@@ -4322,26 +4328,26 @@
       <c r="M51" s="96"/>
     </row>
     <row r="52" spans="1:13" ht="18.399999999999999" customHeight="1">
-      <c r="A52" s="232" t="s">
+      <c r="A52" s="233" t="s">
         <v>120</v>
       </c>
-      <c r="B52" s="234"/>
-      <c r="C52" s="228" t="s">
+      <c r="B52" s="235"/>
+      <c r="C52" s="229" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="229"/>
+      <c r="D52" s="230"/>
       <c r="E52" s="60"/>
-      <c r="F52" s="228" t="s">
+      <c r="F52" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="229"/>
+      <c r="G52" s="230"/>
       <c r="H52" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="I52" s="228" t="s">
+      <c r="I52" s="229" t="s">
         <v>17</v>
       </c>
-      <c r="J52" s="229"/>
+      <c r="J52" s="230"/>
       <c r="K52" s="60"/>
       <c r="L52" s="15"/>
       <c r="M52" s="5"/>
@@ -4496,10 +4502,10 @@
       <c r="M57" s="6"/>
     </row>
     <row r="58" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A58" s="230" t="s">
+      <c r="A58" s="231" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="231"/>
+      <c r="B58" s="232"/>
       <c r="C58" s="98">
         <f>SUMPRODUCT(C53:C57,D53:D57)</f>
         <v>7.75</v>
@@ -4531,27 +4537,27 @@
       <c r="M58" s="96"/>
     </row>
     <row r="59" spans="1:13" ht="18.399999999999999" customHeight="1" thickBot="1">
-      <c r="A59" s="256" t="s">
+      <c r="A59" s="257" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="257"/>
-      <c r="C59" s="257"/>
-      <c r="D59" s="257"/>
-      <c r="E59" s="257"/>
-      <c r="F59" s="257"/>
-      <c r="G59" s="257"/>
-      <c r="H59" s="257"/>
-      <c r="I59" s="257"/>
-      <c r="J59" s="257"/>
-      <c r="K59" s="258"/>
+      <c r="B59" s="258"/>
+      <c r="C59" s="258"/>
+      <c r="D59" s="258"/>
+      <c r="E59" s="258"/>
+      <c r="F59" s="258"/>
+      <c r="G59" s="258"/>
+      <c r="H59" s="258"/>
+      <c r="I59" s="258"/>
+      <c r="J59" s="258"/>
+      <c r="K59" s="259"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
     </row>
     <row r="60" spans="1:13">
-      <c r="A60" s="259" t="s">
+      <c r="A60" s="260" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="260"/>
+      <c r="B60" s="261"/>
       <c r="C60" s="133">
         <f t="shared" ref="C60:J60" si="0">C14+C21+C26+C32+C38+C51+C58</f>
         <v>70.25</v>
@@ -4583,28 +4589,28 @@
       <c r="M60" s="6"/>
     </row>
     <row r="61" spans="1:13" s="97" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A61" s="261" t="s">
+      <c r="A61" s="262" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="262"/>
-      <c r="C61" s="263">
+      <c r="B61" s="263"/>
+      <c r="C61" s="264">
         <f>C60/D60</f>
         <v>0.70250000000000001</v>
       </c>
-      <c r="D61" s="264"/>
-      <c r="E61" s="265"/>
-      <c r="F61" s="266">
+      <c r="D61" s="265"/>
+      <c r="E61" s="266"/>
+      <c r="F61" s="267">
         <f>F60/G60</f>
         <v>0.77800000000000014</v>
       </c>
-      <c r="G61" s="267"/>
-      <c r="H61" s="268"/>
-      <c r="I61" s="269">
+      <c r="G61" s="268"/>
+      <c r="H61" s="269"/>
+      <c r="I61" s="270">
         <f>I60/J60</f>
         <v>0</v>
       </c>
-      <c r="J61" s="270"/>
-      <c r="K61" s="271"/>
+      <c r="J61" s="271"/>
+      <c r="K61" s="272"/>
       <c r="L61" s="136"/>
       <c r="M61" s="136"/>
     </row>
@@ -4679,8 +4685,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A2:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4694,15 +4700,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="272" t="s">
+      <c r="A2" s="273" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="272"/>
-      <c r="C2" s="272"/>
-      <c r="D2" s="272"/>
-      <c r="E2" s="272"/>
-      <c r="F2" s="272"/>
-      <c r="G2" s="272"/>
+      <c r="B2" s="273"/>
+      <c r="C2" s="273"/>
+      <c r="D2" s="273"/>
+      <c r="E2" s="273"/>
+      <c r="F2" s="273"/>
+      <c r="G2" s="273"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="139"/>
@@ -4726,26 +4732,26 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:7" ht="24" thickBot="1">
-      <c r="A6" s="280" t="s">
+      <c r="A6" s="281" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="281"/>
-      <c r="C6" s="281"/>
-      <c r="D6" s="281"/>
-      <c r="E6" s="281"/>
-      <c r="F6" s="281"/>
-      <c r="G6" s="282"/>
+      <c r="B6" s="282"/>
+      <c r="C6" s="282"/>
+      <c r="D6" s="282"/>
+      <c r="E6" s="282"/>
+      <c r="F6" s="282"/>
+      <c r="G6" s="283"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="161" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="283"/>
-      <c r="C7" s="283"/>
-      <c r="D7" s="283"/>
-      <c r="E7" s="283"/>
-      <c r="F7" s="283"/>
-      <c r="G7" s="284"/>
+      <c r="B7" s="284"/>
+      <c r="C7" s="284"/>
+      <c r="D7" s="284"/>
+      <c r="E7" s="284"/>
+      <c r="F7" s="284"/>
+      <c r="G7" s="285"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="210" t="s">
@@ -5030,8 +5036,8 @@
       <c r="A20" s="171" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="285"/>
-      <c r="C20" s="285"/>
+      <c r="B20" s="286"/>
+      <c r="C20" s="286"/>
       <c r="D20" s="223">
         <f>SUM(D9:D19)</f>
         <v>100</v>
@@ -5070,26 +5076,26 @@
       <c r="G22" s="153"/>
     </row>
     <row r="23" spans="1:7" ht="24" thickBot="1">
-      <c r="A23" s="286" t="s">
+      <c r="A23" s="287" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="287"/>
-      <c r="C23" s="287"/>
-      <c r="D23" s="287"/>
-      <c r="E23" s="287"/>
-      <c r="F23" s="287"/>
-      <c r="G23" s="288"/>
+      <c r="B23" s="288"/>
+      <c r="C23" s="288"/>
+      <c r="D23" s="288"/>
+      <c r="E23" s="288"/>
+      <c r="F23" s="288"/>
+      <c r="G23" s="289"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="A24" s="160" t="s">
         <v>136</v>
       </c>
-      <c r="B24" s="273"/>
-      <c r="C24" s="273"/>
-      <c r="D24" s="273"/>
-      <c r="E24" s="273"/>
-      <c r="F24" s="273"/>
-      <c r="G24" s="274"/>
+      <c r="B24" s="274"/>
+      <c r="C24" s="274"/>
+      <c r="D24" s="274"/>
+      <c r="E24" s="274"/>
+      <c r="F24" s="274"/>
+      <c r="G24" s="275"/>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="209" t="s">
@@ -5146,12 +5152,15 @@
         <v>1</v>
       </c>
       <c r="C27" s="142">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D27" s="200">
         <v>8</v>
       </c>
-      <c r="E27" s="200"/>
+      <c r="E27" s="142">
+        <f>B27*C27*D27</f>
+        <v>8</v>
+      </c>
       <c r="F27" s="142" t="s">
         <v>163</v>
       </c>
@@ -5359,12 +5368,12 @@
       </c>
       <c r="E36" s="169">
         <f>SUM(E26:E35)/D36 + E37*D37 + E38*D38 + E39*D39</f>
-        <v>0.49400000000000005</v>
+        <v>0.5515000000000001</v>
       </c>
       <c r="F36" s="169"/>
       <c r="G36" s="170"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" ht="30">
       <c r="A37" s="199" t="s">
         <v>160</v>
       </c>
@@ -5373,13 +5382,19 @@
       <c r="D37" s="203">
         <v>-0.15</v>
       </c>
-      <c r="E37" s="202"/>
-      <c r="F37" s="202"/>
-      <c r="G37" s="204"/>
+      <c r="E37" s="202">
+        <v>0.15</v>
+      </c>
+      <c r="F37" s="228" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="204" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="154" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B38" s="143"/>
       <c r="C38" s="143"/>
@@ -5392,7 +5407,7 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1">
       <c r="A39" s="205" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B39" s="206"/>
       <c r="C39" s="206"/>
@@ -5404,26 +5419,26 @@
       <c r="G39" s="208"/>
     </row>
     <row r="40" spans="1:7" ht="24" thickBot="1">
-      <c r="A40" s="275" t="s">
+      <c r="A40" s="276" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="276"/>
-      <c r="C40" s="276"/>
-      <c r="D40" s="276"/>
-      <c r="E40" s="276"/>
-      <c r="F40" s="276"/>
-      <c r="G40" s="277"/>
+      <c r="B40" s="277"/>
+      <c r="C40" s="277"/>
+      <c r="D40" s="277"/>
+      <c r="E40" s="277"/>
+      <c r="F40" s="277"/>
+      <c r="G40" s="278"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="159" t="s">
         <v>136</v>
       </c>
-      <c r="B41" s="278"/>
-      <c r="C41" s="278"/>
-      <c r="D41" s="278"/>
-      <c r="E41" s="278"/>
-      <c r="F41" s="278"/>
-      <c r="G41" s="279"/>
+      <c r="B41" s="279"/>
+      <c r="C41" s="279"/>
+      <c r="D41" s="279"/>
+      <c r="E41" s="279"/>
+      <c r="F41" s="279"/>
+      <c r="G41" s="280"/>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="178" t="s">
@@ -5450,7 +5465,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="156" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B43" s="145">
         <v>0</v>
@@ -5470,7 +5485,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="175" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B44" s="176">
         <v>0</v>
@@ -5490,7 +5505,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="156" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B45" s="145">
         <v>0</v>
@@ -5510,7 +5525,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="175" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B46" s="176">
         <v>0</v>
@@ -5530,7 +5545,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="156" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B47" s="145">
         <v>0</v>
@@ -5550,7 +5565,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="175" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B48" s="176">
         <v>0</v>
@@ -5570,7 +5585,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="156" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B49" s="145">
         <v>0</v>
@@ -5590,7 +5605,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="175" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B50" s="176">
         <v>0</v>
@@ -5610,7 +5625,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="156" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B51" s="145">
         <v>0</v>
@@ -5630,7 +5645,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="175" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B52" s="176">
         <v>0</v>
@@ -5680,7 +5695,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="156" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B55" s="146"/>
       <c r="C55" s="146"/>
@@ -5693,7 +5708,7 @@
     </row>
     <row r="56" spans="1:7" ht="15.75" thickBot="1">
       <c r="A56" s="185" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B56" s="186"/>
       <c r="C56" s="186"/>
@@ -5734,6 +5749,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B41E0342602C49449CD93109DBCAB8C5" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4cab946e3812a26735e8b0dc00d59aca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3ea4e87-b30d-4ccc-9564-7710f23c54f0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afa808ced5dc9827eedaaa69eb8b35dd" ns2:_="">
     <xsd:import namespace="d3ea4e87-b30d-4ccc-9564-7710f23c54f0"/>
@@ -5865,29 +5889,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1971BE-1E76-44E5-BF52-2DB1BB889C58}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F1A1E89-A0AE-4DED-85B2-2445C39C0F55}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F62C71A-5318-410B-8440-006B73523578}"/>
 </file>
</xml_diff>